<commit_message>
Add missing data from reprocessed sample
</commit_message>
<xml_diff>
--- a/data/Crop biomass C-N content.xlsx
+++ b/data/Crop biomass C-N content.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1063" uniqueCount="613">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="619">
   <si>
     <t>LECO sample ID</t>
   </si>
@@ -1871,13 +1871,31 @@
   </si>
   <si>
     <t>#4 MMNT Y</t>
+  </si>
+  <si>
+    <t>#5 MMNT R</t>
+  </si>
+  <si>
+    <t>#5 MMNT W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#5 MMNT B </t>
+  </si>
+  <si>
+    <t>#5 MMNT Y</t>
+  </si>
+  <si>
+    <t>From archived physical sample reprocessed June 2017</t>
+  </si>
+  <si>
+    <t>From archived physical sample reprocessed June 2017 as validation control</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1895,6 +1913,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1926,7 +1951,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2046,6 +2071,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7242,6 +7277,7 @@
     <mergeCell ref="G32:G39"/>
     <mergeCell ref="F92:F99"/>
     <mergeCell ref="G92:G99"/>
+    <mergeCell ref="G52:G59"/>
     <mergeCell ref="K2:K5"/>
     <mergeCell ref="K6:K9"/>
     <mergeCell ref="K10:K13"/>
@@ -7262,11 +7298,6 @@
     <mergeCell ref="I18:I21"/>
     <mergeCell ref="H18:H21"/>
     <mergeCell ref="G18:G21"/>
-    <mergeCell ref="G52:G59"/>
-    <mergeCell ref="H52:H59"/>
-    <mergeCell ref="I52:I59"/>
-    <mergeCell ref="J52:J59"/>
-    <mergeCell ref="K52:K59"/>
     <mergeCell ref="G22:G23"/>
     <mergeCell ref="H22:H23"/>
     <mergeCell ref="I22:I23"/>
@@ -7297,6 +7328,10 @@
     <mergeCell ref="I48:I51"/>
     <mergeCell ref="J48:J51"/>
     <mergeCell ref="K48:K51"/>
+    <mergeCell ref="H52:H59"/>
+    <mergeCell ref="I52:I59"/>
+    <mergeCell ref="J52:J59"/>
+    <mergeCell ref="K52:K59"/>
     <mergeCell ref="A2:A23"/>
     <mergeCell ref="A24:A51"/>
     <mergeCell ref="A52:A107"/>
@@ -15535,8 +15570,8 @@
   <dimension ref="A1:K245"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A213" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E245" sqref="E245"/>
+      <pane ySplit="1" topLeftCell="A196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E214" sqref="E214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19688,139 +19723,193 @@
       <c r="J205" s="40"/>
       <c r="K205" s="38"/>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A206" s="37"/>
-      <c r="B206" s="2" t="s">
+      <c r="B206" s="47" t="s">
         <v>609</v>
       </c>
-      <c r="C206" s="29"/>
-      <c r="D206" s="29"/>
-      <c r="E206" s="44" t="s">
-        <v>599</v>
-      </c>
-      <c r="F206" s="39">
+      <c r="C206" s="30">
+        <v>2.7587000000000002</v>
+      </c>
+      <c r="D206" s="30">
+        <v>43.953000000000003</v>
+      </c>
+      <c r="E206" s="48" t="s">
+        <v>617</v>
+      </c>
+      <c r="F206" s="46">
         <v>42557</v>
       </c>
-      <c r="G206" s="40" t="s">
-        <v>485</v>
-      </c>
-      <c r="H206" s="40" t="s">
-        <v>485</v>
-      </c>
-      <c r="I206" s="40" t="s">
-        <v>485</v>
-      </c>
-      <c r="J206" s="40" t="s">
-        <v>485</v>
-      </c>
-      <c r="K206" s="38" t="s">
+      <c r="G206" s="45">
+        <f>AVERAGE(C206:C209)</f>
+        <v>2.8782000000000001</v>
+      </c>
+      <c r="H206" s="45">
+        <f>STDEV(C206:C209)</f>
+        <v>0.21251625820157857</v>
+      </c>
+      <c r="I206" s="45">
+        <f>AVERAGE(D206:D209)</f>
+        <v>44.084000000000003</v>
+      </c>
+      <c r="J206" s="45">
+        <f>STDEV(D206:D209)</f>
+        <v>0.17839095642249689</v>
+      </c>
+      <c r="K206" s="45" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="37"/>
-      <c r="B207" s="2" t="s">
-        <v>609</v>
-      </c>
-      <c r="C207" s="29"/>
-      <c r="D207" s="29"/>
-      <c r="E207" s="44"/>
-      <c r="F207" s="39"/>
-      <c r="G207" s="40"/>
-      <c r="H207" s="40"/>
-      <c r="I207" s="40"/>
-      <c r="J207" s="40"/>
-      <c r="K207" s="38"/>
+      <c r="B207" s="47" t="s">
+        <v>610</v>
+      </c>
+      <c r="C207" s="30">
+        <v>3.1145</v>
+      </c>
+      <c r="D207" s="30">
+        <v>44.317</v>
+      </c>
+      <c r="E207" s="48"/>
+      <c r="F207" s="46"/>
+      <c r="G207" s="45"/>
+      <c r="H207" s="45"/>
+      <c r="I207" s="45"/>
+      <c r="J207" s="45"/>
+      <c r="K207" s="45"/>
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="37"/>
-      <c r="B208" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="C208" s="29"/>
-      <c r="D208" s="29"/>
-      <c r="E208" s="44"/>
-      <c r="F208" s="39"/>
-      <c r="G208" s="40"/>
-      <c r="H208" s="40"/>
-      <c r="I208" s="40"/>
-      <c r="J208" s="40"/>
-      <c r="K208" s="38"/>
+      <c r="B208" s="47" t="s">
+        <v>611</v>
+      </c>
+      <c r="C208" s="30">
+        <v>2.6486999999999998</v>
+      </c>
+      <c r="D208" s="30">
+        <v>44.13</v>
+      </c>
+      <c r="E208" s="48"/>
+      <c r="F208" s="46"/>
+      <c r="G208" s="45"/>
+      <c r="H208" s="45"/>
+      <c r="I208" s="45"/>
+      <c r="J208" s="45"/>
+      <c r="K208" s="45"/>
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="37"/>
-      <c r="B209" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="C209" s="29"/>
-      <c r="D209" s="29"/>
-      <c r="E209" s="44"/>
-      <c r="F209" s="39"/>
-      <c r="G209" s="40"/>
-      <c r="H209" s="40"/>
-      <c r="I209" s="40"/>
-      <c r="J209" s="40"/>
-      <c r="K209" s="38"/>
+      <c r="B209" s="47" t="s">
+        <v>612</v>
+      </c>
+      <c r="C209" s="30">
+        <v>2.9908999999999999</v>
+      </c>
+      <c r="D209" s="30">
+        <v>43.936</v>
+      </c>
+      <c r="E209" s="48"/>
+      <c r="F209" s="46"/>
+      <c r="G209" s="45"/>
+      <c r="H209" s="45"/>
+      <c r="I209" s="45"/>
+      <c r="J209" s="45"/>
+      <c r="K209" s="45"/>
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="37"/>
-      <c r="B210" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="C210" s="29"/>
-      <c r="D210" s="29"/>
-      <c r="E210" s="44"/>
-      <c r="F210" s="39"/>
-      <c r="G210" s="40"/>
-      <c r="H210" s="40"/>
-      <c r="I210" s="40"/>
-      <c r="J210" s="40"/>
-      <c r="K210" s="38"/>
+      <c r="B210" s="47" t="s">
+        <v>613</v>
+      </c>
+      <c r="C210" s="30">
+        <v>1.3768</v>
+      </c>
+      <c r="D210" s="30">
+        <v>44.298999999999999</v>
+      </c>
+      <c r="E210" s="48" t="s">
+        <v>618</v>
+      </c>
+      <c r="F210" s="46">
+        <v>42571</v>
+      </c>
+      <c r="G210" s="45">
+        <f>AVERAGE(C210:C213)</f>
+        <v>1.8409499999999999</v>
+      </c>
+      <c r="H210" s="45">
+        <f>STDEV(C210:C213)</f>
+        <v>0.33294024989478244</v>
+      </c>
+      <c r="I210" s="45">
+        <f>AVERAGE(D210:D213)</f>
+        <v>44.335499999999996</v>
+      </c>
+      <c r="J210" s="45">
+        <f>STDEV(D210:D213)</f>
+        <v>0.1820210610524686</v>
+      </c>
+      <c r="K210" s="45" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="37"/>
-      <c r="B211" s="2" t="s">
-        <v>611</v>
-      </c>
-      <c r="C211" s="29"/>
-      <c r="D211" s="29"/>
-      <c r="E211" s="44"/>
-      <c r="F211" s="39"/>
-      <c r="G211" s="40"/>
-      <c r="H211" s="40"/>
-      <c r="I211" s="40"/>
-      <c r="J211" s="40"/>
-      <c r="K211" s="38"/>
+      <c r="B211" s="47" t="s">
+        <v>614</v>
+      </c>
+      <c r="C211" s="30">
+        <v>2.1459999999999999</v>
+      </c>
+      <c r="D211" s="30">
+        <v>44.600999999999999</v>
+      </c>
+      <c r="E211" s="48"/>
+      <c r="F211" s="46"/>
+      <c r="G211" s="45"/>
+      <c r="H211" s="45"/>
+      <c r="I211" s="45"/>
+      <c r="J211" s="45"/>
+      <c r="K211" s="45"/>
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="37"/>
-      <c r="B212" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="C212" s="29"/>
-      <c r="D212" s="29"/>
-      <c r="E212" s="44"/>
-      <c r="F212" s="39"/>
-      <c r="G212" s="40"/>
-      <c r="H212" s="40"/>
-      <c r="I212" s="40"/>
-      <c r="J212" s="40"/>
-      <c r="K212" s="38"/>
+      <c r="B212" s="47" t="s">
+        <v>615</v>
+      </c>
+      <c r="C212" s="30">
+        <v>1.845</v>
+      </c>
+      <c r="D212" s="30">
+        <v>44.247</v>
+      </c>
+      <c r="E212" s="48"/>
+      <c r="F212" s="46"/>
+      <c r="G212" s="45"/>
+      <c r="H212" s="45"/>
+      <c r="I212" s="45"/>
+      <c r="J212" s="45"/>
+      <c r="K212" s="45"/>
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="37"/>
-      <c r="B213" s="2" t="s">
-        <v>612</v>
-      </c>
-      <c r="C213" s="29"/>
-      <c r="D213" s="29"/>
-      <c r="E213" s="44"/>
-      <c r="F213" s="39"/>
-      <c r="G213" s="40"/>
-      <c r="H213" s="40"/>
-      <c r="I213" s="40"/>
-      <c r="J213" s="40"/>
-      <c r="K213" s="38"/>
+      <c r="B213" s="47" t="s">
+        <v>616</v>
+      </c>
+      <c r="C213" s="30">
+        <v>1.996</v>
+      </c>
+      <c r="D213" s="30">
+        <v>44.195</v>
+      </c>
+      <c r="E213" s="48"/>
+      <c r="F213" s="46"/>
+      <c r="G213" s="45"/>
+      <c r="H213" s="45"/>
+      <c r="I213" s="45"/>
+      <c r="J213" s="45"/>
+      <c r="K213" s="45"/>
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="37"/>
@@ -20463,7 +20552,14 @@
       <c r="K245" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="185">
+  <mergeCells count="192">
+    <mergeCell ref="G206:G209"/>
+    <mergeCell ref="H206:H209"/>
+    <mergeCell ref="I206:I209"/>
+    <mergeCell ref="J206:J209"/>
+    <mergeCell ref="K206:K209"/>
+    <mergeCell ref="F206:F209"/>
+    <mergeCell ref="E210:E213"/>
     <mergeCell ref="F238:F245"/>
     <mergeCell ref="G238:G245"/>
     <mergeCell ref="H238:H245"/>
@@ -20484,19 +20580,19 @@
     <mergeCell ref="J230:J237"/>
     <mergeCell ref="K230:K237"/>
     <mergeCell ref="K198:K205"/>
-    <mergeCell ref="F206:F213"/>
-    <mergeCell ref="G206:G213"/>
-    <mergeCell ref="H206:H213"/>
-    <mergeCell ref="I206:I213"/>
-    <mergeCell ref="J206:J213"/>
-    <mergeCell ref="K206:K213"/>
     <mergeCell ref="F214:F221"/>
     <mergeCell ref="G214:G221"/>
     <mergeCell ref="H214:H221"/>
     <mergeCell ref="I214:I221"/>
     <mergeCell ref="J214:J221"/>
     <mergeCell ref="K214:K221"/>
-    <mergeCell ref="E206:E213"/>
+    <mergeCell ref="E206:E209"/>
+    <mergeCell ref="F210:F213"/>
+    <mergeCell ref="G210:G213"/>
+    <mergeCell ref="H210:H213"/>
+    <mergeCell ref="I210:I213"/>
+    <mergeCell ref="J210:J213"/>
+    <mergeCell ref="K210:K213"/>
     <mergeCell ref="F182:F189"/>
     <mergeCell ref="G182:G189"/>
     <mergeCell ref="H182:H189"/>
@@ -20509,6 +20605,7 @@
     <mergeCell ref="I190:I197"/>
     <mergeCell ref="J190:J197"/>
     <mergeCell ref="K190:K197"/>
+    <mergeCell ref="F94:F101"/>
     <mergeCell ref="F198:F205"/>
     <mergeCell ref="G198:G205"/>
     <mergeCell ref="H198:H205"/>
@@ -20519,7 +20616,29 @@
     <mergeCell ref="H80:H86"/>
     <mergeCell ref="I80:I86"/>
     <mergeCell ref="J80:J86"/>
-    <mergeCell ref="K80:K86"/>
+    <mergeCell ref="F174:F181"/>
+    <mergeCell ref="F102:F109"/>
+    <mergeCell ref="F110:F117"/>
+    <mergeCell ref="F126:F133"/>
+    <mergeCell ref="F134:F141"/>
+    <mergeCell ref="F142:F149"/>
+    <mergeCell ref="F150:F157"/>
+    <mergeCell ref="F118:F125"/>
+    <mergeCell ref="G174:G181"/>
+    <mergeCell ref="H174:H181"/>
+    <mergeCell ref="I174:I181"/>
+    <mergeCell ref="J174:J181"/>
+    <mergeCell ref="G118:G125"/>
+    <mergeCell ref="F158:F165"/>
+    <mergeCell ref="K134:K141"/>
+    <mergeCell ref="K142:K149"/>
+    <mergeCell ref="J142:J149"/>
+    <mergeCell ref="I142:I149"/>
+    <mergeCell ref="H142:H149"/>
+    <mergeCell ref="G142:G149"/>
+    <mergeCell ref="G126:G133"/>
+    <mergeCell ref="G134:G141"/>
+    <mergeCell ref="H134:H141"/>
     <mergeCell ref="F166:F169"/>
     <mergeCell ref="F170:F173"/>
     <mergeCell ref="G166:G169"/>
@@ -20532,17 +20651,6 @@
     <mergeCell ref="I170:I173"/>
     <mergeCell ref="H170:H173"/>
     <mergeCell ref="G170:G173"/>
-    <mergeCell ref="F158:F165"/>
-    <mergeCell ref="K134:K141"/>
-    <mergeCell ref="K142:K149"/>
-    <mergeCell ref="J142:J149"/>
-    <mergeCell ref="I142:I149"/>
-    <mergeCell ref="H142:H149"/>
-    <mergeCell ref="G142:G149"/>
-    <mergeCell ref="G126:G133"/>
-    <mergeCell ref="G134:G141"/>
-    <mergeCell ref="H134:H141"/>
-    <mergeCell ref="F174:F181"/>
     <mergeCell ref="F2:F9"/>
     <mergeCell ref="F10:F17"/>
     <mergeCell ref="F18:F25"/>
@@ -20552,18 +20660,6 @@
     <mergeCell ref="F52:F65"/>
     <mergeCell ref="F66:F79"/>
     <mergeCell ref="F87:F93"/>
-    <mergeCell ref="F94:F101"/>
-    <mergeCell ref="F102:F109"/>
-    <mergeCell ref="F110:F117"/>
-    <mergeCell ref="F126:F133"/>
-    <mergeCell ref="F134:F141"/>
-    <mergeCell ref="F142:F149"/>
-    <mergeCell ref="F150:F157"/>
-    <mergeCell ref="F118:F125"/>
-    <mergeCell ref="G174:G181"/>
-    <mergeCell ref="H174:H181"/>
-    <mergeCell ref="I174:I181"/>
-    <mergeCell ref="J174:J181"/>
     <mergeCell ref="K174:K181"/>
     <mergeCell ref="J150:J157"/>
     <mergeCell ref="K150:K157"/>
@@ -20575,9 +20671,6 @@
     <mergeCell ref="G150:G157"/>
     <mergeCell ref="H150:H157"/>
     <mergeCell ref="I150:I157"/>
-    <mergeCell ref="G118:G125"/>
-    <mergeCell ref="H118:H125"/>
-    <mergeCell ref="I118:I125"/>
     <mergeCell ref="I134:I141"/>
     <mergeCell ref="J134:J141"/>
     <mergeCell ref="K126:K133"/>
@@ -20587,6 +20680,7 @@
     <mergeCell ref="K118:K125"/>
     <mergeCell ref="H102:H109"/>
     <mergeCell ref="I102:I109"/>
+    <mergeCell ref="H118:H125"/>
     <mergeCell ref="K94:K101"/>
     <mergeCell ref="K102:K109"/>
     <mergeCell ref="J118:J125"/>
@@ -20601,6 +20695,8 @@
     <mergeCell ref="I110:I117"/>
     <mergeCell ref="H110:H117"/>
     <mergeCell ref="K110:K117"/>
+    <mergeCell ref="I118:I125"/>
+    <mergeCell ref="K80:K86"/>
     <mergeCell ref="J2:J9"/>
     <mergeCell ref="G10:G17"/>
     <mergeCell ref="H10:H17"/>

</xml_diff>